<commit_message>
Actualización en los CSV de las URLS de los sets
</commit_message>
<xml_diff>
--- a/Archivos CSV/urls imagenes Cloudinary peso reducido.xlsx
+++ b/Archivos CSV/urls imagenes Cloudinary peso reducido.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvargasp\Documents\Archivos MAAJI\Archivos CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A80F37-579C-4E66-A158-EA865FF29424}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1290153F-2AF7-4C14-9F79-6CE2C7767E15}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{FAF58B75-BD7C-45FF-AD1B-561300509A0B}"/>
   </bookViews>
@@ -1942,9 +1942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98BB106-48B0-4DED-8950-C24559FCBB89}">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>